<commit_message>
model helper to control predictions: individual, chain, multi
</commit_message>
<xml_diff>
--- a/results_overview.xlsx
+++ b/results_overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Desktop\code\grambank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72906883-0178-4FC7-A058-ACD7B379AB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438568E2-6C55-4316-A193-8A461D8D6B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="1830" windowWidth="10540" windowHeight="11400" xr2:uid="{653932A9-A32F-4DE4-972A-82852F470DFA}"/>
+    <workbookView xWindow="3780" yWindow="3290" windowWidth="15990" windowHeight="11400" xr2:uid="{653932A9-A32F-4DE4-972A-82852F470DFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87867E31-F8EF-49BC-ADBF-4142799607B0}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fininshed the addition of cluster data and run experiments
</commit_message>
<xml_diff>
--- a/results_overview.xlsx
+++ b/results_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Desktop\code\grambank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438568E2-6C55-4316-A193-8A461D8D6B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DA1513-21BC-4B88-B0C0-FB1169FEE3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="3290" windowWidth="15990" windowHeight="11400" xr2:uid="{653932A9-A32F-4DE4-972A-82852F470DFA}"/>
+    <workbookView xWindow="-870" yWindow="1180" windowWidth="13120" windowHeight="11400" xr2:uid="{653932A9-A32F-4DE4-972A-82852F470DFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="23">
   <si>
     <t>model</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>feat+fam(1hot-enc)</t>
+  </si>
+  <si>
+    <t>feat+kmeans</t>
+  </si>
+  <si>
+    <t>feat+dbscan</t>
+  </si>
+  <si>
+    <t>feat+hdbscan</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87867E31-F8EF-49BC-ADBF-4142799607B0}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,18 +522,18 @@
     <col min="1" max="1" width="20.54296875" customWidth="1"/>
     <col min="2" max="2" width="18.26953125" customWidth="1"/>
     <col min="3" max="3" width="8.90625" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" customWidth="1"/>
-    <col min="9" max="10" width="18.6328125" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" customWidth="1"/>
-    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="4" max="7" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" customWidth="1"/>
+    <col min="10" max="13" width="12.1796875" customWidth="1"/>
+    <col min="14" max="14" width="19.453125" customWidth="1"/>
+    <col min="15" max="19" width="18.6328125" customWidth="1"/>
+    <col min="20" max="20" width="19.54296875" customWidth="1"/>
+    <col min="21" max="21" width="17.7265625" customWidth="1"/>
+    <col min="22" max="22" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,34 +547,61 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="U1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -579,13 +615,13 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -597,16 +633,43 @@
         <v>18</v>
       </c>
       <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
         <v>10</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" t="s">
+      <c r="V3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -646,8 +709,35 @@
       <c r="M4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -660,13 +750,13 @@
       <c r="D5">
         <v>0.3</v>
       </c>
-      <c r="E5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="E5">
+        <v>0.3</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
         <v>0.3</v>
       </c>
       <c r="H5" s="4">
@@ -678,18 +768,45 @@
       <c r="J5" s="4">
         <v>0.3</v>
       </c>
-      <c r="K5">
-        <v>0.3</v>
-      </c>
-      <c r="L5">
-        <v>0.3</v>
-      </c>
-      <c r="M5">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.4">
+      <c r="K5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="R5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="T5">
+        <v>0.3</v>
+      </c>
+      <c r="U5">
+        <v>0.3</v>
+      </c>
+      <c r="V5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -703,29 +820,56 @@
         <v>0.51600000000000001</v>
       </c>
       <c r="E7">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="H7">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>0.76100000000000001</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>0.70099999999999996</v>
       </c>
-      <c r="H7">
+      <c r="K7">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="L7">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="M7">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="N7">
         <v>0.65300000000000002</v>
       </c>
-      <c r="I7">
+      <c r="O7">
         <v>0.69</v>
       </c>
-      <c r="J7">
+      <c r="P7">
         <v>0.64300000000000002</v>
       </c>
-      <c r="K7">
+      <c r="Q7">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="R7">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="S7">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="T7">
         <v>0.748</v>
       </c>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.4">
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -739,29 +883,56 @@
         <v>0.66800000000000004</v>
       </c>
       <c r="E8">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="F8">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="G8">
         <v>0.67200000000000004</v>
       </c>
-      <c r="F8">
+      <c r="H8">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="I8">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>0.67700000000000005</v>
       </c>
-      <c r="H8">
+      <c r="K8">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L8">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="M8">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="N8">
         <v>0.66100000000000003</v>
       </c>
-      <c r="I8">
+      <c r="O8">
         <v>0.67400000000000004</v>
       </c>
-      <c r="J8">
+      <c r="P8">
         <v>0.66100000000000003</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="R8">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="S8">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="T8">
         <v>0.71099999999999997</v>
       </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.35">
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -775,29 +946,56 @@
         <v>0.64100000000000001</v>
       </c>
       <c r="E9">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0.64</v>
+      </c>
+      <c r="G9">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="H9">
         <v>0.69899999999999995</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>0.74299999999999999</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>0.70399999999999996</v>
       </c>
-      <c r="H9">
+      <c r="K9">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="L9">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="M9">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="N9">
         <v>0.68899999999999995</v>
       </c>
-      <c r="I9">
+      <c r="O9">
         <v>0.70299999999999996</v>
       </c>
-      <c r="J9">
+      <c r="P9">
         <v>0.68700000000000006</v>
       </c>
-      <c r="K9">
+      <c r="Q9">
+        <v>0.69</v>
+      </c>
+      <c r="R9">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="S9">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="T9">
         <v>0.64500000000000002</v>
       </c>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.4">
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -811,29 +1009,56 @@
         <v>0.499</v>
       </c>
       <c r="E10">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.497</v>
+      </c>
+      <c r="G10">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="H10">
         <v>0.70599999999999996</v>
       </c>
-      <c r="F10">
+      <c r="I10">
         <v>0.76600000000000001</v>
       </c>
-      <c r="G10">
+      <c r="J10">
         <v>0.71099999999999997</v>
       </c>
-      <c r="H10">
+      <c r="K10">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="L10">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="M10">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="N10">
         <v>0.66600000000000004</v>
       </c>
-      <c r="I10">
+      <c r="O10">
         <v>0.70199999999999996</v>
       </c>
-      <c r="J10">
+      <c r="P10">
         <v>0.65600000000000003</v>
       </c>
-      <c r="K10">
+      <c r="Q10">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="R10">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="S10">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="T10">
         <v>0.72499999999999998</v>
       </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.4">
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -847,29 +1072,56 @@
         <v>0.51300000000000001</v>
       </c>
       <c r="E11">
+        <v>0.505</v>
+      </c>
+      <c r="F11">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="H11">
         <v>0.67300000000000004</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>0.73099999999999998</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>0.67900000000000005</v>
       </c>
-      <c r="H11">
+      <c r="K11">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="L11">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="M11">
+        <v>0.69</v>
+      </c>
+      <c r="N11">
         <v>0.64200000000000002</v>
       </c>
-      <c r="I11">
+      <c r="O11">
         <v>0.67200000000000004</v>
       </c>
-      <c r="J11">
+      <c r="P11">
         <v>0.63500000000000001</v>
       </c>
-      <c r="K11">
+      <c r="Q11">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="R11">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="S11">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="T11">
         <v>0.65600000000000003</v>
       </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.4">
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -883,32 +1135,59 @@
         <v>0.51600000000000001</v>
       </c>
       <c r="E12">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="H12">
         <v>0.69499999999999995</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <v>0.76100000000000001</v>
       </c>
-      <c r="G12">
+      <c r="J12">
         <v>0.70099999999999996</v>
       </c>
-      <c r="H12" s="4">
+      <c r="K12">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="L12">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="M12">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="N12" s="4">
         <v>0.65300000000000002</v>
       </c>
-      <c r="I12" s="4">
+      <c r="O12" s="4">
         <v>0.69</v>
       </c>
-      <c r="J12" s="4">
+      <c r="P12" s="4">
         <v>0.64300000000000002</v>
       </c>
-      <c r="K12">
+      <c r="Q12" s="4">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="T12">
         <v>0.748</v>
       </c>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="U12" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>